<commit_message>
NEW Optimization + ATP Synthase/PMF
</commit_message>
<xml_diff>
--- a/FRR_with_ATP_synthase_Model_PQT_1_PCT_1_FDT_1_rqr_500_and_buffer/LaiskY.xlsx
+++ b/FRR_with_ATP_synthase_Model_PQT_1_PCT_1_FDT_1_rqr_500_and_buffer/LaiskY.xlsx
@@ -8,17 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/GitHub/Laisk-PSII/FRR_with_ATP_synthase_Model_PQT_1_PCT_1_FDT_1_rqr_500_and_buffer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CF1181A2-A6ED-EC4C-9820-2DA766643042}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{65ECD8BD-AB73-1C4F-95A6-6AD340A9E4E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8220" yWindow="460" windowWidth="14360" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ys" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1287,8 +1295,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D136"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1485,6 +1493,7 @@
         <v>12</v>
       </c>
       <c r="B12">
+        <f>E12/100</f>
         <v>0</v>
       </c>
       <c r="C12">
@@ -1502,6 +1511,7 @@
         <v>13</v>
       </c>
       <c r="B13">
+        <f t="shared" ref="B13:B76" si="0">E13/100</f>
         <v>0</v>
       </c>
       <c r="C13">
@@ -1519,6 +1529,7 @@
         <v>14</v>
       </c>
       <c r="B14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C14">
@@ -1536,6 +1547,7 @@
         <v>15</v>
       </c>
       <c r="B15">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C15">
@@ -1553,6 +1565,7 @@
         <v>16</v>
       </c>
       <c r="B16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C16">
@@ -1570,6 +1583,7 @@
         <v>17</v>
       </c>
       <c r="B17">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C17">
@@ -1587,6 +1601,7 @@
         <v>18</v>
       </c>
       <c r="B18">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C18">
@@ -1604,10 +1619,12 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <f>E19*100</f>
+        <v>25</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1621,9 +1638,11 @@
         <v>20</v>
       </c>
       <c r="B20">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C20">
+        <f t="shared" ref="C20:C83" si="1">E20*100</f>
         <v>0</v>
       </c>
       <c r="D20">
@@ -1638,9 +1657,11 @@
         <v>21</v>
       </c>
       <c r="B21">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C21">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D21">
@@ -1655,9 +1676,11 @@
         <v>22</v>
       </c>
       <c r="B22">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C22">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D22">
@@ -1672,9 +1695,11 @@
         <v>23</v>
       </c>
       <c r="B23">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C23">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D23">
@@ -1689,9 +1714,11 @@
         <v>24</v>
       </c>
       <c r="B24">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C24">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D24">
@@ -1706,9 +1733,11 @@
         <v>25</v>
       </c>
       <c r="B25">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C25">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D25">
@@ -1723,9 +1752,11 @@
         <v>26</v>
       </c>
       <c r="B26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C26">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D26">
@@ -1740,9 +1771,11 @@
         <v>27</v>
       </c>
       <c r="B27">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C27">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D27">
@@ -1757,9 +1790,11 @@
         <v>28</v>
       </c>
       <c r="B28">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C28">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D28">
@@ -1774,9 +1809,11 @@
         <v>29</v>
       </c>
       <c r="B29">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C29">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D29">
@@ -1791,9 +1828,11 @@
         <v>30</v>
       </c>
       <c r="B30">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C30">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D30">
@@ -1808,9 +1847,11 @@
         <v>31</v>
       </c>
       <c r="B31">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C31">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D31">
@@ -1825,9 +1866,11 @@
         <v>32</v>
       </c>
       <c r="B32">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C32">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D32">
@@ -1842,9 +1885,11 @@
         <v>33</v>
       </c>
       <c r="B33">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C33">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D33">
@@ -1859,9 +1904,11 @@
         <v>34</v>
       </c>
       <c r="B34">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C34">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D34">
@@ -1876,9 +1923,11 @@
         <v>35</v>
       </c>
       <c r="B35">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C35">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D35">
@@ -1893,9 +1942,11 @@
         <v>36</v>
       </c>
       <c r="B36">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C36">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D36">
@@ -1910,9 +1961,11 @@
         <v>37</v>
       </c>
       <c r="B37">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C37">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D37">
@@ -1927,9 +1980,11 @@
         <v>38</v>
       </c>
       <c r="B38">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C38">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D38">
@@ -1944,9 +1999,11 @@
         <v>39</v>
       </c>
       <c r="B39">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C39">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D39">
@@ -1961,9 +2018,11 @@
         <v>40</v>
       </c>
       <c r="B40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D40">
@@ -1978,9 +2037,11 @@
         <v>41</v>
       </c>
       <c r="B41">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C41">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D41">
@@ -1995,9 +2056,11 @@
         <v>42</v>
       </c>
       <c r="B42">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C42">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D42">
@@ -2012,10 +2075,12 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>75</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -2029,9 +2094,11 @@
         <v>44</v>
       </c>
       <c r="B44">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C44">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D44">
@@ -2046,9 +2113,11 @@
         <v>45</v>
       </c>
       <c r="B45">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C45">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D45">
@@ -2063,9 +2132,11 @@
         <v>46</v>
       </c>
       <c r="B46">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C46">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D46">
@@ -2080,9 +2151,11 @@
         <v>47</v>
       </c>
       <c r="B47">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C47">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D47">
@@ -2097,9 +2170,11 @@
         <v>48</v>
       </c>
       <c r="B48">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C48">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D48">
@@ -2114,9 +2189,11 @@
         <v>49</v>
       </c>
       <c r="B49">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C49">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D49">
@@ -2131,9 +2208,11 @@
         <v>50</v>
       </c>
       <c r="B50">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C50">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D50">
@@ -2148,9 +2227,11 @@
         <v>51</v>
       </c>
       <c r="B51">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C51">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D51">
@@ -2165,9 +2246,11 @@
         <v>52</v>
       </c>
       <c r="B52">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C52">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D52">
@@ -2182,9 +2265,11 @@
         <v>53</v>
       </c>
       <c r="B53">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C53">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D53">
@@ -2199,9 +2284,11 @@
         <v>54</v>
       </c>
       <c r="B54">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C54">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D54">
@@ -2216,9 +2303,11 @@
         <v>55</v>
       </c>
       <c r="B55">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C55">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D55">
@@ -2233,9 +2322,11 @@
         <v>56</v>
       </c>
       <c r="B56">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C56">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D56">
@@ -2250,9 +2341,11 @@
         <v>57</v>
       </c>
       <c r="B57">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C57">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D57">
@@ -2267,9 +2360,11 @@
         <v>58</v>
       </c>
       <c r="B58">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C58">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D58">
@@ -2284,9 +2379,11 @@
         <v>59</v>
       </c>
       <c r="B59">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C59">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D59">
@@ -2301,9 +2398,11 @@
         <v>60</v>
       </c>
       <c r="B60">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C60">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D60">
@@ -2318,9 +2417,11 @@
         <v>61</v>
       </c>
       <c r="B61">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C61">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D61">
@@ -2335,9 +2436,11 @@
         <v>62</v>
       </c>
       <c r="B62">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C62">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D62">
@@ -2352,9 +2455,11 @@
         <v>63</v>
       </c>
       <c r="B63">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D63">
@@ -2369,9 +2474,11 @@
         <v>64</v>
       </c>
       <c r="B64">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C64">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D64">
@@ -2386,9 +2493,11 @@
         <v>65</v>
       </c>
       <c r="B65">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C65">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D65">
@@ -2403,9 +2512,11 @@
         <v>66</v>
       </c>
       <c r="B66">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C66">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D66">
@@ -2420,9 +2531,11 @@
         <v>67</v>
       </c>
       <c r="B67">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C67">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D67">
@@ -2437,9 +2550,11 @@
         <v>68</v>
       </c>
       <c r="B68">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C68">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D68">
@@ -2454,9 +2569,11 @@
         <v>69</v>
       </c>
       <c r="B69">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C69">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D69">
@@ -2471,9 +2588,11 @@
         <v>70</v>
       </c>
       <c r="B70">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C70">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D70">
@@ -2488,9 +2607,11 @@
         <v>71</v>
       </c>
       <c r="B71">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C71">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D71">
@@ -2505,9 +2626,11 @@
         <v>72</v>
       </c>
       <c r="B72">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C72">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D72">
@@ -2522,9 +2645,11 @@
         <v>73</v>
       </c>
       <c r="B73">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C73">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D73">
@@ -2539,9 +2664,11 @@
         <v>74</v>
       </c>
       <c r="B74">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C74">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D74">
@@ -2556,9 +2683,11 @@
         <v>75</v>
       </c>
       <c r="B75">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C75">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D75">
@@ -2573,9 +2702,11 @@
         <v>76</v>
       </c>
       <c r="B76">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C76">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D76">
@@ -2590,9 +2721,11 @@
         <v>77</v>
       </c>
       <c r="B77">
+        <f t="shared" ref="B77:B136" si="2">E77/100</f>
         <v>0</v>
       </c>
       <c r="C77">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D77">
@@ -2607,9 +2740,11 @@
         <v>78</v>
       </c>
       <c r="B78">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C78">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D78">
@@ -2624,9 +2759,11 @@
         <v>79</v>
       </c>
       <c r="B79">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C79">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D79">
@@ -2641,9 +2778,11 @@
         <v>80</v>
       </c>
       <c r="B80">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C80">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D80">
@@ -2658,9 +2797,11 @@
         <v>81</v>
       </c>
       <c r="B81">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C81">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D81">
@@ -2675,9 +2816,11 @@
         <v>82</v>
       </c>
       <c r="B82">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C82">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D82">
@@ -2692,9 +2835,11 @@
         <v>83</v>
       </c>
       <c r="B83">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C83">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D83">
@@ -2709,9 +2854,11 @@
         <v>84</v>
       </c>
       <c r="B84">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C84">
+        <f t="shared" ref="C84:C136" si="3">E84*100</f>
         <v>0</v>
       </c>
       <c r="D84">
@@ -2726,9 +2873,11 @@
         <v>85</v>
       </c>
       <c r="B85">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C85">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D85">
@@ -2743,9 +2892,11 @@
         <v>86</v>
       </c>
       <c r="B86">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C86">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D86">
@@ -2760,9 +2911,11 @@
         <v>87</v>
       </c>
       <c r="B87">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C87">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D87">
@@ -2777,9 +2930,11 @@
         <v>88</v>
       </c>
       <c r="B88">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C88">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D88">
@@ -2794,9 +2949,11 @@
         <v>89</v>
       </c>
       <c r="B89">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C89">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D89">
@@ -2811,9 +2968,11 @@
         <v>90</v>
       </c>
       <c r="B90">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C90">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D90">
@@ -2828,9 +2987,11 @@
         <v>91</v>
       </c>
       <c r="B91">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C91">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D91">
@@ -2845,9 +3006,11 @@
         <v>92</v>
       </c>
       <c r="B92">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C92">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D92">
@@ -2862,9 +3025,11 @@
         <v>93</v>
       </c>
       <c r="B93">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C93">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D93">
@@ -2879,9 +3044,11 @@
         <v>94</v>
       </c>
       <c r="B94">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C94">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D94">
@@ -2896,9 +3063,11 @@
         <v>95</v>
       </c>
       <c r="B95">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C95">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D95">
@@ -2913,9 +3082,11 @@
         <v>96</v>
       </c>
       <c r="B96">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C96">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D96">
@@ -2930,9 +3101,11 @@
         <v>97</v>
       </c>
       <c r="B97">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C97">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D97">
@@ -2947,9 +3120,11 @@
         <v>98</v>
       </c>
       <c r="B98">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C98">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D98">
@@ -2964,10 +3139,12 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.04</v>
       </c>
       <c r="C99">
-        <v>50</v>
+        <f t="shared" si="3"/>
+        <v>400</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -2981,9 +3158,11 @@
         <v>100</v>
       </c>
       <c r="B100">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C100">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D100">
@@ -2998,9 +3177,11 @@
         <v>101</v>
       </c>
       <c r="B101">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C101">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D101">
@@ -3015,9 +3196,11 @@
         <v>102</v>
       </c>
       <c r="B102">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C102">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D102">
@@ -3032,9 +3215,11 @@
         <v>103</v>
       </c>
       <c r="B103">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C103">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D103">
@@ -3049,9 +3234,11 @@
         <v>104</v>
       </c>
       <c r="B104">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C104">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D104">
@@ -3066,10 +3253,12 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C105">
-        <v>50</v>
+        <f t="shared" si="3"/>
+        <v>700</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -3083,9 +3272,11 @@
         <v>106</v>
       </c>
       <c r="B106">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C106">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D106">
@@ -3100,9 +3291,11 @@
         <v>107</v>
       </c>
       <c r="B107">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C107">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D107">
@@ -3117,10 +3310,12 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="C108">
-        <v>50</v>
+        <f t="shared" si="3"/>
+        <v>10000</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -3134,10 +3329,12 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.04</v>
       </c>
       <c r="C109">
-        <v>50</v>
+        <f t="shared" si="3"/>
+        <v>400</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -3151,9 +3348,11 @@
         <v>110</v>
       </c>
       <c r="B110">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C110">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D110">
@@ -3168,10 +3367,12 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="C111">
-        <v>100</v>
+        <f t="shared" si="3"/>
+        <v>10000</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -3185,10 +3386,12 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="C112">
-        <v>100</v>
+        <f t="shared" si="3"/>
+        <v>10000</v>
       </c>
       <c r="D112">
         <v>1</v>
@@ -3202,9 +3405,11 @@
         <v>113</v>
       </c>
       <c r="B113">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C113">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D113">
@@ -3219,10 +3424,12 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.3</v>
       </c>
       <c r="C114">
-        <v>50</v>
+        <f t="shared" si="3"/>
+        <v>3000</v>
       </c>
       <c r="D114">
         <v>1</v>
@@ -3236,10 +3443,12 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="C115">
-        <v>50</v>
+        <f t="shared" si="3"/>
+        <v>10000</v>
       </c>
       <c r="D115">
         <v>1</v>
@@ -3253,9 +3462,11 @@
         <v>116</v>
       </c>
       <c r="B116">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C116">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D116">
@@ -3270,10 +3481,12 @@
         <v>117</v>
       </c>
       <c r="B117">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C117">
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="D117">
         <v>1</v>
@@ -3287,10 +3500,12 @@
         <v>118</v>
       </c>
       <c r="B118">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.1</v>
       </c>
       <c r="C118">
-        <v>50</v>
+        <f t="shared" si="3"/>
+        <v>1000</v>
       </c>
       <c r="D118">
         <v>1</v>
@@ -3304,9 +3519,11 @@
         <v>119</v>
       </c>
       <c r="B119">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C119">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D119">
@@ -3321,9 +3538,11 @@
         <v>120</v>
       </c>
       <c r="B120">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C120">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D120">
@@ -3338,9 +3557,11 @@
         <v>121</v>
       </c>
       <c r="B121">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C121">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D121">
@@ -3355,9 +3576,11 @@
         <v>122</v>
       </c>
       <c r="B122">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C122">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D122">
@@ -3372,9 +3595,11 @@
         <v>123</v>
       </c>
       <c r="B123">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C123">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D123">
@@ -3389,9 +3614,11 @@
         <v>124</v>
       </c>
       <c r="B124">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C124">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D124">
@@ -3406,9 +3633,11 @@
         <v>125</v>
       </c>
       <c r="B125">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C125">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D125">
@@ -3423,9 +3652,11 @@
         <v>126</v>
       </c>
       <c r="B126">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C126">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D126">
@@ -3440,9 +3671,11 @@
         <v>127</v>
       </c>
       <c r="B127">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C127">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D127">
@@ -3457,13 +3690,15 @@
         <v>128</v>
       </c>
       <c r="B128">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C128">
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="D128">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E128">
         <v>0</v>
@@ -3474,13 +3709,15 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.1</v>
       </c>
       <c r="C129">
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>1000</v>
       </c>
       <c r="D129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E129">
         <v>10</v>
@@ -3491,13 +3728,15 @@
         <v>130</v>
       </c>
       <c r="B130">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.1</v>
       </c>
       <c r="C130">
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>1000</v>
       </c>
       <c r="D130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E130">
         <v>10</v>
@@ -3508,13 +3747,15 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>100</v>
       </c>
       <c r="C131">
-        <v>100</v>
+        <f t="shared" si="3"/>
+        <v>1000000</v>
       </c>
       <c r="D131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E131">
         <v>10000</v>
@@ -3525,13 +3766,15 @@
         <v>132</v>
       </c>
       <c r="B132">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1E-3</v>
       </c>
       <c r="C132">
-        <v>0.1</v>
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
       <c r="D132">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E132">
         <v>0.1</v>
@@ -3542,13 +3785,15 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.1</v>
       </c>
       <c r="C133">
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>1000</v>
       </c>
       <c r="D133">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E133">
         <v>10</v>
@@ -3559,13 +3804,15 @@
         <v>134</v>
       </c>
       <c r="B134">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.1</v>
       </c>
       <c r="C134">
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>1000</v>
       </c>
       <c r="D134">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E134">
         <v>10</v>
@@ -3576,13 +3823,15 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>100</v>
       </c>
       <c r="C135">
-        <v>100</v>
+        <f t="shared" si="3"/>
+        <v>1000000</v>
       </c>
       <c r="D135">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E135">
         <v>10000</v>
@@ -3593,13 +3842,15 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1E-3</v>
       </c>
       <c r="C136">
-        <v>0.1</v>
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
       <c r="D136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E136">
         <v>0.1</v>

</xml_diff>